<commit_message>
updated formatting of T3 output to match manuscript table
Ran end to end

updated readme documentation
</commit_message>
<xml_diff>
--- a/Publication/Outputs/Tables/T3.xlsx
+++ b/Publication/Outputs/Tables/T3.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">Category: Variable: Stratified Variable</t>
   </si>
@@ -23,7 +23,7 @@
     <t xml:space="preserve">AT Initiated Post-Stroke* (n = 35)</t>
   </si>
   <si>
-    <t xml:space="preserve">p value†</t>
+    <t xml:space="preserve">p-value†</t>
   </si>
   <si>
     <t xml:space="preserve">Total (N = 52)</t>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">30 [17–56]</t>
   </si>
   <si>
-    <t xml:space="preserve">0.00</t>
+    <t xml:space="preserve">8E-6</t>
   </si>
   <si>
     <t xml:space="preserve">48 [24–161]</t>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t xml:space="preserve">AT Choice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   AT Choice</t>
   </si>
   <si>
     <t xml:space="preserve">   ASA (81 mg, PO)</t>
@@ -645,100 +642,83 @@
         <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
         <v>28</v>
-      </c>
-      <c r="C13" t="s">
-        <v>42</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>